<commit_message>
Updated db design and tracker
</commit_message>
<xml_diff>
--- a/database_design.xlsx
+++ b/database_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPL\Legacy&amp;Looms\code_base\legacy-and-looms-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8886E5-7BFE-4F6D-8D44-9321D55CD86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B8D52D-E05B-41BC-8B54-264AA176A0A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="party" sheetId="2" r:id="rId1"/>
@@ -702,7 +702,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA29B30E-A5BB-48A4-AC5B-359E03EF12FC}">
   <dimension ref="B2:AP23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:D16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1079,7 @@
   <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1245,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D6"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1320,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1465,7 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1582,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1664,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB70A2E7-131E-45F9-8330-41EB8C47BF5B}">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,7 +1845,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4053C0-B343-4A8B-A2F7-BDE10FF1CCE2}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2130,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2454,7 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,7 +2629,7 @@
   <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>